<commit_message>
Claryfy “Split surrogate pairs” feature.
</commit_message>
<xml_diff>
--- a/RegexFeatureMatrix.xlsx
+++ b/RegexFeatureMatrix.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feature Matrix" sheetId="1" r:id="R08fca6251a1a49a3"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feature Matrix" sheetId="1" r:id="R39eba9c3c1824f02"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -1215,6 +1215,12 @@
     <x:t>Empty set</x:t>
   </x:si>
   <x:si>
+    <x:t>Split surrogates</x:t>
+  </x:si>
+  <x:si>
+    <x:t>“.” matches the components of surrogate pairs</x:t>
+  </x:si>
+  <x:si>
     <x:t>Fuzzy matching</x:t>
   </x:si>
   <x:si>
@@ -41122,29 +41128,29 @@
       <x:c r="B210" s="5" t="s">
         <x:v>396</x:v>
       </x:c>
-      <x:c r="C210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="D210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="G210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="H210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="I210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="J210" t="s">
-        <x:v>1</x:v>
+      <x:c r="C210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="D210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="E210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="F210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="G210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="H210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="I210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="J210" s="6" t="s">
+        <x:v>73</x:v>
       </x:c>
       <x:c r="K210" t="s">
         <x:v>1</x:v>
@@ -41152,44 +41158,44 @@
       <x:c r="L210" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="M210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="N210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="O210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="P210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="Q210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="R210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="S210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="T210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="U210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="V210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="W210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="X210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="Y210" t="s">
-        <x:v>1</x:v>
+      <x:c r="M210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="N210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="O210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="P210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="Q210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="R210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="S210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="T210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="U210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="V210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="W210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="X210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="Y210" s="6" t="s">
+        <x:v>73</x:v>
       </x:c>
       <x:c r="Z210" t="s">
         <x:v>1</x:v>
@@ -41224,8 +41230,8 @@
       <x:c r="AJ210" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="AK210" t="s">
-        <x:v>1</x:v>
+      <x:c r="AK210" s="6" t="s">
+        <x:v>73</x:v>
       </x:c>
       <x:c r="AL210" t="s">
         <x:v>1</x:v>
@@ -41233,29 +41239,29 @@
       <x:c r="AM210" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="AN210" t="s">
-        <x:v>1</x:v>
+      <x:c r="AN210" s="6" t="s">
+        <x:v>73</x:v>
       </x:c>
       <x:c r="AO210" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="AP210" t="s">
-        <x:v>1</x:v>
+      <x:c r="AP210" s="6" t="s">
+        <x:v>73</x:v>
       </x:c>
       <x:c r="AQ210" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="AR210" t="s">
-        <x:v>1</x:v>
+      <x:c r="AR210" s="6" t="s">
+        <x:v>73</x:v>
       </x:c>
       <x:c r="AS210" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="AT210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AU210" s="6" t="s">
-        <x:v>73</x:v>
+      <x:c r="AT210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="AU210" t="s">
+        <x:v>1</x:v>
       </x:c>
       <x:c r="AV210" t="s">
         <x:v>1</x:v>
@@ -41287,11 +41293,11 @@
       <x:c r="BE210" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="BF210" s="6" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="BG210" s="6" t="s">
-        <x:v>73</x:v>
+      <x:c r="BF210" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BG210" t="s">
+        <x:v>1</x:v>
       </x:c>
       <x:c r="BH210" t="s">
         <x:v>1</x:v>
@@ -41302,11 +41308,11 @@
       <x:c r="BJ210" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="BK210" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BL210" t="s">
-        <x:v>1</x:v>
+      <x:c r="BK210" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="BL210" s="6" t="s">
+        <x:v>73</x:v>
       </x:c>
       <x:c r="BM210" s="6" t="s">
         <x:v>73</x:v>
@@ -41319,205 +41325,408 @@
       </x:c>
     </x:row>
     <x:row r="211">
-      <x:c r="A211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="D211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="E211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="F211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="G211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="H211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="I211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="J211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="K211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="L211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="M211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="N211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="O211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="P211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="Q211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="R211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="S211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="T211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="U211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="V211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="W211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="X211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="Y211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="Z211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AA211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AB211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AC211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AD211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AE211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AF211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AG211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AH211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AI211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AJ211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AK211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AL211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AM211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AN211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AO211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AP211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AQ211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AR211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AS211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AT211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AU211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AV211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AW211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AX211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AY211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="AZ211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BA211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BB211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BC211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BD211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BE211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BF211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BG211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BH211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BI211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BJ211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BK211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BL211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BM211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BN211" s="7" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="BO211" s="7" t="s">
+      <x:c r="A211" s="4" t="s">
+        <x:v>397</x:v>
+      </x:c>
+      <x:c r="B211" s="5" t="s">
+        <x:v>398</x:v>
+      </x:c>
+      <x:c r="C211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="H211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="J211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="K211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="L211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="M211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="N211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="O211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="P211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="Q211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="R211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="S211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="T211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="U211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="W211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="X211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="Y211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="Z211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AA211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AB211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AC211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AD211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AE211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AF211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AG211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AH211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AI211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AJ211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AK211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AL211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AM211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AN211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AO211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AP211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AQ211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AR211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AS211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AT211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AU211" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="AV211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AW211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AX211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AY211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AZ211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BA211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BB211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BC211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BD211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BE211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BF211" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="BG211" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="BH211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BI211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BJ211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BK211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BL211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BM211" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="BN211" s="6" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="BO211" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="212">
+      <x:c r="A212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="G212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="H212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="J212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="K212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="L212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="M212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="N212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="O212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="P212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="Q212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="R212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="S212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="T212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="U212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="V212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="W212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="X212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="Y212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="Z212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AA212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AB212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AC212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AD212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AE212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AF212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AG212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AH212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AI212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AJ212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AK212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AL212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AM212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AN212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AO212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AP212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AQ212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AR212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AS212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AT212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AU212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AV212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AW212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AX212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AY212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="AZ212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BA212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BB212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BC212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BD212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BE212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BF212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BG212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BH212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BI212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BJ212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BK212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BL212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BM212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BN212" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="BO212" s="7" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Clarify Feature Matrix for TRegEx.
</commit_message>
<xml_diff>
--- a/RegexFeatureMatrix.xlsx
+++ b/RegexFeatureMatrix.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feature Matrix" sheetId="1" r:id="R72f47f07c39b4a33"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feature Matrix" sheetId="1" r:id="R3e0f4aab41954a56"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -106,7 +106,7 @@
 15.2.0</x:t>
   </x:si>
   <x:si>
-    <x:t>VCL (C++Builder, Delphi)
+    <x:t>TRegEx (C++Builder, Delphi)
 29.0</x:t>
   </x:si>
   <x:si>
@@ -248,7 +248,7 @@
     <x:t>Regex (Jeyemhex)</x:t>
   </x:si>
   <x:si>
-    <x:t>VCL (C++Builder, Delphi)</x:t>
+    <x:t>TRegEx (C++Builder, Delphi)</x:t>
   </x:si>
   <x:si>
     <x:t>General</x:t>
@@ -1434,7 +1434,7 @@
     <x:col min="66" max="66" width="9.4" customWidth="1"/>
     <x:col min="67" max="67" width="11.393" customWidth="1"/>
     <x:col min="68" max="68" width="11.89" customWidth="1"/>
-    <x:col min="69" max="69" width="22.283" customWidth="1"/>
+    <x:col min="69" max="69" width="25.281" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" ht="49" customHeight="1">

</xml_diff>